<commit_message>
2024 participant update + correction
</commit_message>
<xml_diff>
--- a/agreement_participants/emerald/agr_participants_emerald_current.xlsx
+++ b/agreement_participants/emerald/agr_participants_emerald_current.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">agr_name</t>
   </si>
@@ -50,64 +50,97 @@
     <t xml:space="preserve">emerald</t>
   </si>
   <si>
-    <t xml:space="preserve">Departementenes Sikkerhets- Og Serviceorganisasjon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dss</t>
+    <t xml:space="preserve">Handelshøyskolen BI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi</t>
   </si>
   <si>
     <t xml:space="preserve">Emerald Publishing</t>
   </si>
   <si>
-    <t xml:space="preserve">Emerald 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handelshøyskolen BI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Høgskolen i Gjøvik</t>
+    <t xml:space="preserve">Emerald 2023-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høgskolen I Innlandet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høgskolen i Innlandet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høgskolen i Molde - Vitenskapelig høgskole i logistikk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">himolde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høgskolen i Østfold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hioef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høgskulen På Vestlandet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hvl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høgskulen på Vestlandet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høyskolen Kristiania - Ernst G Mortensens Stiftelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Høyskolen Kristiania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasjonalbiblioteket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nofima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nofima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOFIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nord Universitet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nord universitet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norges Handelshøyskole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nhh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norges teknisk-naturvitenskapelige universitet</t>
   </si>
   <si>
     <t xml:space="preserve">ntnu</t>
   </si>
   <si>
-    <t xml:space="preserve">Norges teknisk-naturvitenskapelige universitet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Høgskolen i Sør Trøndelag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasjonalbiblioteket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nofima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nofima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOFIMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nord Universitet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nord universitet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norges Handelshøyskole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nhh</t>
+    <t xml:space="preserve">ntnu_1920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Olavs Hospital HF</t>
   </si>
   <si>
     <t xml:space="preserve">OsloMet - Storbyuniversitetet</t>
@@ -137,6 +170,12 @@
     <t xml:space="preserve">UiT Norges arktiske universitet</t>
   </si>
   <si>
+    <t xml:space="preserve">uit_1902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universitetssykehuset Nord-Norge HF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Universitetet I Stavanger</t>
   </si>
   <si>
@@ -146,16 +185,19 @@
     <t xml:space="preserve">Universitetet i Stavanger</t>
   </si>
   <si>
+    <t xml:space="preserve">Universitetet I Sørøst-Norge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universitetet i Sørøst-Norge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Universitetet i Agder</t>
   </si>
   <si>
     <t xml:space="preserve">uia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universitetet i Bergen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uib</t>
   </si>
 </sst>
 </file>
@@ -540,10 +582,14 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2"/>
-      <c r="E2"/>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="n">
+        <v>158</v>
+      </c>
       <c r="F2" t="n">
-        <v>15361</v>
+        <v>15353</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -552,13 +598,13 @@
         <v>15</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="3">
@@ -572,13 +618,13 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" t="n">
-        <v>158</v>
+        <v>209</v>
       </c>
       <c r="F3" t="n">
-        <v>15353</v>
+        <v>15428</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -587,13 +633,13 @@
         <v>15</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="4">
@@ -601,19 +647,19 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="n">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="F4" t="n">
-        <v>15507</v>
+        <v>15435</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -622,13 +668,13 @@
         <v>15</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="5">
@@ -639,16 +685,16 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="n">
-        <v>194</v>
+        <v>224</v>
       </c>
       <c r="F5" t="n">
-        <v>15507</v>
+        <v>15443</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -657,13 +703,13 @@
         <v>15</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="6">
@@ -671,19 +717,19 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E6" t="n">
-        <v>5931</v>
+        <v>203</v>
       </c>
       <c r="F6" t="n">
-        <v>15471</v>
+        <v>15449</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -692,13 +738,13 @@
         <v>15</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="7">
@@ -706,19 +752,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" t="n">
-        <v>7543</v>
+        <v>1615</v>
       </c>
       <c r="F7" t="n">
-        <v>15496</v>
+        <v>15444</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -727,13 +773,13 @@
         <v>15</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="8">
@@ -741,19 +787,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
       <c r="E8" t="n">
-        <v>204</v>
+        <v>5931</v>
       </c>
       <c r="F8" t="n">
-        <v>15499</v>
+        <v>15471</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -762,13 +808,13 @@
         <v>15</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="9">
@@ -776,19 +822,19 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E9" t="n">
-        <v>191</v>
+        <v>7543</v>
       </c>
       <c r="F9" t="n">
-        <v>15480</v>
+        <v>15496</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -797,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="10">
@@ -811,19 +857,19 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" t="n">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="F10" t="n">
-        <v>15439</v>
+        <v>15499</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -832,13 +878,13 @@
         <v>15</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="11">
@@ -846,19 +892,19 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>37</v>
       </c>
       <c r="E11" t="n">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="F11" t="n">
-        <v>15550</v>
+        <v>15480</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -867,13 +913,13 @@
         <v>15</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="12">
@@ -881,19 +927,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" t="n">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F12" t="n">
-        <v>15552</v>
+        <v>15507</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -902,13 +948,13 @@
         <v>15</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="13">
@@ -916,19 +962,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" t="n">
-        <v>217</v>
+        <v>1920</v>
       </c>
       <c r="F13" t="n">
-        <v>15551</v>
+        <v>15507</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
@@ -937,13 +983,13 @@
         <v>15</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="14">
@@ -951,19 +997,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
       <c r="E14" t="n">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="F14" t="n">
-        <v>15548</v>
+        <v>15439</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -972,13 +1018,13 @@
         <v>15</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="15">
@@ -992,13 +1038,13 @@
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E15" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F15" t="n">
-        <v>15549</v>
+        <v>15550</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1007,13 +1053,188 @@
         <v>15</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>42005</v>
+        <v>44927</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>42369</v>
+        <v>46022</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>45368</v>
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="n">
+        <v>186</v>
+      </c>
+      <c r="F16" t="n">
+        <v>15552</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1902</v>
+      </c>
+      <c r="F17" t="n">
+        <v>15552</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="n">
+        <v>217</v>
+      </c>
+      <c r="F18" t="n">
+        <v>15551</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="n">
+        <v>222</v>
+      </c>
+      <c r="F19" t="n">
+        <v>15447</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="n">
+        <v>201</v>
+      </c>
+      <c r="F20" t="n">
+        <v>15548</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>46022</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>45369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>